<commit_message>
add averages into results report
</commit_message>
<xml_diff>
--- a/docs/logs-13-03-2019_18-15-51/log-conv_time-13-03-2019_18-15-51.xlsx
+++ b/docs/logs-13-03-2019_18-15-51/log-conv_time-13-03-2019_18-15-51.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\AsposePoC\docs\logs-13-03-2019_18-15-51\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C6F2CD-A0D5-421D-8B29-8C82A6864181}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B1D847-4AF7-498F-A216-EB9BE3A2EA36}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="174">
   <si>
     <t>Time</t>
   </si>
@@ -542,6 +542,15 @@
   </si>
   <si>
     <t xml:space="preserve"> XSLX 2016.xlsx</t>
+  </si>
+  <si>
+    <t>Average All</t>
+  </si>
+  <si>
+    <t>Average Slow</t>
+  </si>
+  <si>
+    <t>Average Fast</t>
   </si>
 </sst>
 </file>
@@ -1025,9 +1034,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1386,7 +1396,7 @@
   <dimension ref="A1:G163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32:F32"/>
+      <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1419,45 +1429,45 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43537.761041666665</v>
+        <v>43537.761180555557</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="C2">
-        <v>2838</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>2858</v>
+        <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43537.761053240742</v>
+        <v>43537.761041666665</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>814</v>
+        <v>2838</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F3">
-        <v>827</v>
+        <v>2858</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
@@ -1468,19 +1478,19 @@
         <v>43537.761053240742</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4">
-        <v>105</v>
+        <v>814</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E4">
         <v>11</v>
       </c>
       <c r="F4">
-        <v>121</v>
+        <v>827</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
@@ -1491,19 +1501,19 @@
         <v>43537.761053240742</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5">
-        <v>251</v>
+        <v>105</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E5">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F5">
-        <v>259</v>
+        <v>121</v>
       </c>
       <c r="G5" t="s">
         <v>8</v>
@@ -1511,13 +1521,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>43537.761064814818</v>
+        <v>43537.761053240742</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6">
-        <v>296</v>
+        <v>251</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -1526,7 +1536,7 @@
         <v>6</v>
       </c>
       <c r="F6">
-        <v>304</v>
+        <v>259</v>
       </c>
       <c r="G6" t="s">
         <v>8</v>
@@ -1537,19 +1547,19 @@
         <v>43537.761064814818</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7">
-        <v>22</v>
+        <v>296</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F7">
-        <v>36</v>
+        <v>304</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>
@@ -1557,22 +1567,22 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>43537.761076388888</v>
+        <v>43537.761064814818</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8">
-        <v>1339</v>
+        <v>22</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E8">
         <v>11</v>
       </c>
       <c r="F8">
-        <v>1352</v>
+        <v>36</v>
       </c>
       <c r="G8" t="s">
         <v>8</v>
@@ -1583,10 +1593,10 @@
         <v>43537.761076388888</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9">
-        <v>22</v>
+        <v>1339</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -1595,7 +1605,7 @@
         <v>11</v>
       </c>
       <c r="F9">
-        <v>35</v>
+        <v>1352</v>
       </c>
       <c r="G9" t="s">
         <v>8</v>
@@ -1606,19 +1616,19 @@
         <v>43537.761076388888</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10">
-        <v>127</v>
+        <v>22</v>
       </c>
       <c r="D10">
         <v>2</v>
       </c>
       <c r="E10">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F10">
-        <v>139</v>
+        <v>35</v>
       </c>
       <c r="G10" t="s">
         <v>8</v>
@@ -1629,10 +1639,10 @@
         <v>43537.761076388888</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11">
-        <v>75</v>
+        <v>127</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -1641,7 +1651,7 @@
         <v>10</v>
       </c>
       <c r="F11">
-        <v>87</v>
+        <v>139</v>
       </c>
       <c r="G11" t="s">
         <v>8</v>
@@ -1649,22 +1659,22 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>43537.761087962965</v>
+        <v>43537.761076388888</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12">
-        <v>203</v>
+        <v>75</v>
       </c>
       <c r="D12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E12">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F12">
-        <v>214</v>
+        <v>87</v>
       </c>
       <c r="G12" t="s">
         <v>8</v>
@@ -1675,19 +1685,19 @@
         <v>43537.761087962965</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E13">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F13">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="G13" t="s">
         <v>8</v>
@@ -1698,10 +1708,10 @@
         <v>43537.761087962965</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14">
-        <v>281</v>
+        <v>193</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -1710,7 +1720,7 @@
         <v>10</v>
       </c>
       <c r="F14">
-        <v>293</v>
+        <v>205</v>
       </c>
       <c r="G14" t="s">
         <v>8</v>
@@ -1721,19 +1731,19 @@
         <v>43537.761087962965</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15">
-        <v>204</v>
+        <v>281</v>
       </c>
       <c r="D15">
         <v>2</v>
       </c>
       <c r="E15">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15">
-        <v>217</v>
+        <v>293</v>
       </c>
       <c r="G15" t="s">
         <v>8</v>
@@ -1744,10 +1754,10 @@
         <v>43537.761087962965</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16">
-        <v>38</v>
+        <v>204</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -1756,7 +1766,7 @@
         <v>11</v>
       </c>
       <c r="F16">
-        <v>51</v>
+        <v>217</v>
       </c>
       <c r="G16" t="s">
         <v>8</v>
@@ -1764,22 +1774,22 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>43537.761099537034</v>
+        <v>43537.761087962965</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17">
-        <v>115</v>
+        <v>38</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F17">
-        <v>126</v>
+        <v>51</v>
       </c>
       <c r="G17" t="s">
         <v>8</v>
@@ -1790,19 +1800,19 @@
         <v>43537.761099537034</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18">
-        <v>540</v>
+        <v>115</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F18">
-        <v>549</v>
+        <v>126</v>
       </c>
       <c r="G18" t="s">
         <v>8</v>
@@ -1810,22 +1820,22 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>43537.761111111111</v>
+        <v>43537.761099537034</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19">
-        <v>438</v>
+        <v>540</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F19">
-        <v>449</v>
+        <v>549</v>
       </c>
       <c r="G19" t="s">
         <v>8</v>
@@ -1836,19 +1846,19 @@
         <v>43537.761111111111</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20">
-        <v>209</v>
+        <v>438</v>
       </c>
       <c r="D20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20">
         <v>10</v>
       </c>
       <c r="F20">
-        <v>221</v>
+        <v>449</v>
       </c>
       <c r="G20" t="s">
         <v>8</v>
@@ -1859,19 +1869,19 @@
         <v>43537.761111111111</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21">
-        <v>18</v>
+        <v>209</v>
       </c>
       <c r="D21">
         <v>2</v>
       </c>
       <c r="E21">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F21">
-        <v>31</v>
+        <v>221</v>
       </c>
       <c r="G21" t="s">
         <v>8</v>
@@ -1882,19 +1892,19 @@
         <v>43537.761111111111</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22">
-        <v>247</v>
+        <v>18</v>
       </c>
       <c r="D22">
         <v>2</v>
       </c>
       <c r="E22">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F22">
-        <v>259</v>
+        <v>31</v>
       </c>
       <c r="G22" t="s">
         <v>8</v>
@@ -1905,19 +1915,19 @@
         <v>43537.761111111111</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E23">
         <v>10</v>
       </c>
       <c r="F23">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="G23" t="s">
         <v>8</v>
@@ -1925,22 +1935,22 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>43537.761122685188</v>
+        <v>43537.761111111111</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24">
-        <v>58</v>
+        <v>244</v>
       </c>
       <c r="D24">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="E24">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F24">
-        <v>92</v>
+        <v>255</v>
       </c>
       <c r="G24" t="s">
         <v>8</v>
@@ -1948,22 +1958,22 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>43537.761134259257</v>
+        <v>43537.761122685188</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25">
-        <v>1379</v>
+        <v>58</v>
       </c>
       <c r="D25">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E25">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F25">
-        <v>1391</v>
+        <v>92</v>
       </c>
       <c r="G25" t="s">
         <v>8</v>
@@ -1974,19 +1984,19 @@
         <v>43537.761134259257</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C26">
-        <v>35</v>
+        <v>1379</v>
       </c>
       <c r="D26">
         <v>2</v>
       </c>
       <c r="E26">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F26">
-        <v>49</v>
+        <v>1391</v>
       </c>
       <c r="G26" t="s">
         <v>8</v>
@@ -1994,22 +2004,22 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>43537.76116898148</v>
+        <v>43537.761134259257</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C27">
-        <v>2561</v>
+        <v>35</v>
       </c>
       <c r="D27">
         <v>2</v>
       </c>
       <c r="E27">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F27">
-        <v>2573</v>
+        <v>49</v>
       </c>
       <c r="G27" t="s">
         <v>8</v>
@@ -2020,19 +2030,19 @@
         <v>43537.76116898148</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28">
-        <v>377</v>
+        <v>2561</v>
       </c>
       <c r="D28">
         <v>2</v>
       </c>
       <c r="E28">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F28">
-        <v>390</v>
+        <v>2573</v>
       </c>
       <c r="G28" t="s">
         <v>8</v>
@@ -2043,19 +2053,19 @@
         <v>43537.76116898148</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29">
-        <v>391</v>
+        <v>377</v>
       </c>
       <c r="D29">
         <v>2</v>
       </c>
       <c r="E29">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F29">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="G29" t="s">
         <v>8</v>
@@ -2063,22 +2073,22 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>43537.761180555557</v>
+        <v>43537.76116898148</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C30">
-        <v>279</v>
+        <v>391</v>
       </c>
       <c r="D30">
         <v>2</v>
       </c>
       <c r="E30">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F30">
-        <v>287</v>
+        <v>400</v>
       </c>
       <c r="G30" t="s">
         <v>8</v>
@@ -2089,19 +2099,19 @@
         <v>43537.761180555557</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C31">
-        <v>13</v>
+        <v>279</v>
       </c>
       <c r="D31">
         <v>2</v>
       </c>
       <c r="E31">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F31">
-        <v>26</v>
+        <v>287</v>
       </c>
       <c r="G31" t="s">
         <v>8</v>
@@ -2112,22 +2122,22 @@
         <v>43537.761180555557</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C32">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F32">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="G32" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -5144,6 +5154,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G163">
+    <sortCondition ref="G2:G163"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5153,7 +5166,7 @@
   <dimension ref="A1:I162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F2" sqref="F2:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5231,7 +5244,10 @@
       <c r="G3" t="s">
         <v>8</v>
       </c>
-      <c r="I3">
+      <c r="H3" t="s">
+        <v>171</v>
+      </c>
+      <c r="I3" s="2">
         <f>AVERAGE(F2:F162)</f>
         <v>248.06211180124222</v>
       </c>
@@ -5258,6 +5274,13 @@
       <c r="G4" t="s">
         <v>8</v>
       </c>
+      <c r="H4" t="s">
+        <v>172</v>
+      </c>
+      <c r="I4" s="2">
+        <f>AVERAGE(F2:F7)</f>
+        <v>2810.6666666666665</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -5281,6 +5304,13 @@
       <c r="G5" t="s">
         <v>8</v>
       </c>
+      <c r="H5" t="s">
+        <v>173</v>
+      </c>
+      <c r="I5" s="2">
+        <f>AVERAGE(F8:F162)</f>
+        <v>148.86451612903227</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -8894,8 +8924,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G163">
-    <sortCondition descending="1" ref="F2:F163"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G162">
+    <sortCondition ref="G2:G162"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>